<commit_message>
corregido la hoja de calculo de la práctica
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Carlos.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Carlos.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="40">
   <si>
     <t>GP</t>
   </si>
@@ -423,13 +423,19 @@
     <t>Dirección del proyecto</t>
   </si>
   <si>
-    <t>Diseño de la BD</t>
-  </si>
-  <si>
     <t>Familiarización con la herramienta GitHub</t>
   </si>
   <si>
     <t>Entrega de la propuesta del proyecto</t>
+  </si>
+  <si>
+    <t>Implementación base</t>
+  </si>
+  <si>
+    <t>Práctica de auditoria</t>
+  </si>
+  <si>
+    <t>Diseño del esquema E/R de la BD</t>
   </si>
 </sst>
 </file>
@@ -1323,40 +1329,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFCCFFFF"/>
           <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCFFFF"/>
-          <bgColor rgb="FFCCFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF99CCFF"/>
-          <bgColor rgb="FF99CCFF"/>
         </patternFill>
       </fill>
       <border>
@@ -1803,10 +1781,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.75</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1896,11 +1874,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77606272"/>
-        <c:axId val="77617024"/>
+        <c:axId val="82132352"/>
+        <c:axId val="82151296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77606272"/>
+        <c:axId val="82132352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1936,13 +1914,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77617024"/>
+        <c:crossAx val="82151296"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77617024"/>
+        <c:axId val="82151296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1993,7 +1971,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77606272"/>
+        <c:crossAx val="82132352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2014,7 +1992,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5000,12 +4978,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="28" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7833,12 +7811,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10617,12 +10595,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13450,12 +13428,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13677,7 +13655,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>9.25</v>
+        <v>13.25</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -13689,11 +13667,11 @@
       </c>
       <c r="J6" s="116">
         <f>Mar!G35</f>
-        <v>4.75</v>
+        <v>5.25</v>
       </c>
       <c r="K6" s="116">
         <f>Abr!G36</f>
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
@@ -14234,12 +14212,12 @@
     <row r="39" ht="15.75" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G7">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16733,12 +16711,12 @@
     <mergeCell ref="AO1:AP1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G32">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G32">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16752,7 +16730,7 @@
   <dimension ref="A1:BC42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G4"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -17019,7 +16997,7 @@
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
       <c r="AR3" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AS3" s="22">
         <v>1</v>
@@ -17198,7 +17176,7 @@
       </c>
       <c r="G6" s="15">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="23"/>
@@ -17212,7 +17190,7 @@
       <c r="Q6" s="23"/>
       <c r="R6" s="23"/>
       <c r="S6" s="23">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="T6" s="23"/>
       <c r="U6" s="19"/>
@@ -17266,7 +17244,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G7" s="15">
         <f t="shared" si="0"/>
@@ -17338,7 +17316,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="15">
         <f t="shared" si="0"/>
@@ -18966,7 +18944,7 @@
       </c>
       <c r="G35" s="36">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>5.25</v>
       </c>
       <c r="H35" s="37">
         <f t="shared" ref="H35:AL35" si="1">SUM(H3:H34)</f>
@@ -19014,7 +18992,7 @@
       </c>
       <c r="S35" s="72">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="T35" s="72">
         <f t="shared" si="1"/>
@@ -19527,12 +19505,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G34">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G34">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19546,7 +19524,7 @@
   <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -19822,14 +19800,24 @@
     </row>
     <row r="4" spans="1:54" ht="13.5" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="B4" s="21">
+        <v>85</v>
+      </c>
+      <c r="C4" s="23">
+        <v>2</v>
+      </c>
+      <c r="D4" s="23">
+        <v>54</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>37</v>
+      </c>
       <c r="G4" s="15">
-        <f t="shared" ref="G3:G36" si="1">SUM(H4:AK4)</f>
-        <v>0</v>
+        <f t="shared" ref="G4:G36" si="1">SUM(H4:AK4)</f>
+        <v>0.5</v>
       </c>
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
@@ -19841,7 +19829,9 @@
       <c r="O4" s="23"/>
       <c r="P4" s="23"/>
       <c r="Q4" s="23"/>
-      <c r="R4" s="19"/>
+      <c r="R4" s="19">
+        <v>0.5</v>
+      </c>
       <c r="S4" s="19"/>
       <c r="T4" s="23"/>
       <c r="U4" s="23"/>
@@ -19881,14 +19871,24 @@
     </row>
     <row r="5" spans="1:54" ht="13.5" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="21">
+        <v>85</v>
+      </c>
+      <c r="C5" s="23">
+        <v>2</v>
+      </c>
+      <c r="D5" s="23">
+        <v>54</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>37</v>
+      </c>
       <c r="G5" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
@@ -19901,7 +19901,9 @@
       <c r="P5" s="23"/>
       <c r="Q5" s="23"/>
       <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
+      <c r="S5" s="19">
+        <v>1</v>
+      </c>
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
       <c r="V5" s="23"/>
@@ -19940,14 +19942,24 @@
     </row>
     <row r="6" spans="1:54" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="21">
+        <v>85</v>
+      </c>
+      <c r="C6" s="23">
+        <v>2</v>
+      </c>
+      <c r="D6" s="23">
+        <v>44</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>38</v>
+      </c>
       <c r="G6" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -19963,7 +19975,9 @@
       <c r="S6" s="19"/>
       <c r="T6" s="23"/>
       <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
+      <c r="V6" s="23">
+        <v>2</v>
+      </c>
       <c r="W6" s="23"/>
       <c r="X6" s="23"/>
       <c r="Y6" s="19"/>
@@ -21719,7 +21733,7 @@
       </c>
       <c r="G36" s="36">
         <f t="shared" si="1"/>
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="H36" s="37">
         <f t="shared" ref="H36:AK36" si="2">SUM(H3:H35)</f>
@@ -21763,11 +21777,11 @@
       </c>
       <c r="R36" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S36" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T36" s="72">
         <f t="shared" si="2"/>
@@ -21779,7 +21793,7 @@
       </c>
       <c r="V36" s="72">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W36" s="72">
         <f t="shared" si="2"/>
@@ -22269,22 +22283,22 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25055,12 +25069,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27783,12 +27797,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30560,12 +30574,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33336,12 +33350,12 @@
     <mergeCell ref="AR1:AS1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36064,12 +36078,12 @@
     <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G35">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
hoja de esfuerzos actualizada
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Carlos.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Carlos.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="42">
   <si>
     <t>GP</t>
   </si>
@@ -432,13 +432,16 @@
     <t>Implementación base</t>
   </si>
   <si>
-    <t>Práctica de auditoria</t>
-  </si>
-  <si>
     <t>Diseño del esquema E/R de la BD</t>
   </si>
   <si>
     <t>Reunión para el reparto de tareas</t>
+  </si>
+  <si>
+    <t>Primera parte de la auditoría interna</t>
+  </si>
+  <si>
+    <t>Práctica de auditoría</t>
   </si>
 </sst>
 </file>
@@ -1787,7 +1790,7 @@
                   <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1877,11 +1880,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="90918272"/>
-        <c:axId val="90937216"/>
+        <c:axId val="94915968"/>
+        <c:axId val="94934912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90918272"/>
+        <c:axId val="94915968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1917,13 +1920,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90937216"/>
+        <c:crossAx val="94934912"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90937216"/>
+        <c:axId val="94934912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1974,7 +1977,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90918272"/>
+        <c:crossAx val="94915968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1995,7 +1998,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -13658,7 +13661,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>14.25</v>
+        <v>14.75</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -13674,7 +13677,7 @@
       </c>
       <c r="K6" s="116">
         <f>Abr!G36</f>
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
@@ -16733,7 +16736,7 @@
   <dimension ref="A1:BC42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -17247,7 +17250,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="15">
         <f t="shared" si="0"/>
@@ -19527,7 +19530,7 @@
   <dimension ref="A1:BB43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -19958,7 +19961,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G6" s="15">
         <f t="shared" si="1"/>
@@ -20029,7 +20032,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G7" s="15">
         <f t="shared" si="1"/>
@@ -20087,14 +20090,24 @@
     </row>
     <row r="8" spans="1:54" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="21">
+        <v>85</v>
+      </c>
+      <c r="C8" s="23">
+        <v>2</v>
+      </c>
+      <c r="D8" s="23">
+        <v>44</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="G8" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
@@ -20121,7 +20134,9 @@
       <c r="AD8" s="19"/>
       <c r="AE8" s="19"/>
       <c r="AF8" s="19"/>
-      <c r="AG8" s="19"/>
+      <c r="AG8" s="19">
+        <v>0.5</v>
+      </c>
       <c r="AH8" s="23"/>
       <c r="AI8" s="23"/>
       <c r="AJ8" s="23"/>
@@ -21748,7 +21763,7 @@
       </c>
       <c r="G36" s="36">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="H36" s="37">
         <f t="shared" ref="H36:AK36" si="2">SUM(H3:H35)</f>
@@ -21852,7 +21867,7 @@
       </c>
       <c r="AG36" s="37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AH36" s="72">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Elaboración del "tríptico" para la presentación comercial
</commit_message>
<xml_diff>
--- a/team/efforts/Recopilacion_Esfuerzos_Carlos.xlsx
+++ b/team/efforts/Recopilacion_Esfuerzos_Carlos.xlsx
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="49">
   <si>
     <t>GP</t>
   </si>
@@ -457,6 +457,12 @@
   </si>
   <si>
     <t>55.4</t>
+  </si>
+  <si>
+    <t>Reunión para repartir tareas</t>
+  </si>
+  <si>
+    <t>Elaboración del tríptico para la presentación</t>
   </si>
 </sst>
 </file>
@@ -1771,11 +1777,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="es-ES"/>
               <a:t>Gráfica Esfuerzos totales/Formación</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1813,7 +1821,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1900,11 +1908,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="103716736"/>
-        <c:axId val="103735296"/>
+        <c:axId val="94610176"/>
+        <c:axId val="94612480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103716736"/>
+        <c:axId val="94610176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1923,11 +1931,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="es-ES"/>
                   <a:t>Mes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -1940,13 +1950,13 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103735296"/>
+        <c:crossAx val="94612480"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103735296"/>
+        <c:axId val="94612480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1974,11 +1984,13 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="es-ES"/>
                   <a:t>Horas</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1997,7 +2009,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103716736"/>
+        <c:crossAx val="94610176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2009,6 +2021,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
@@ -2019,7 +2032,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -14262,7 +14275,7 @@
       </c>
       <c r="G6" s="114">
         <f t="shared" ref="G6:G7" si="0">SUM(H6:S6)</f>
-        <v>17.75</v>
+        <v>21</v>
       </c>
       <c r="H6" s="116">
         <f>Ene!G36</f>
@@ -14282,7 +14295,7 @@
       </c>
       <c r="L6" s="116">
         <f>May!G36</f>
-        <v>2.5</v>
+        <v>5.75</v>
       </c>
       <c r="M6" s="116">
         <f>Jun!G36</f>
@@ -17338,7 +17351,7 @@
   <dimension ref="A1:BC42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="AR3" sqref="AR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -22948,7 +22961,7 @@
   <dimension ref="A1:BC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -23375,14 +23388,24 @@
     </row>
     <row r="6" spans="1:55" ht="13.5" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="21">
+        <v>84</v>
+      </c>
+      <c r="C6" s="23">
+        <v>2</v>
+      </c>
+      <c r="D6" s="23">
+        <v>53</v>
+      </c>
+      <c r="E6" s="24">
+        <v>1</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>47</v>
+      </c>
       <c r="G6" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
@@ -23397,7 +23420,9 @@
       <c r="R6" s="23"/>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
+      <c r="U6" s="23">
+        <v>0.75</v>
+      </c>
       <c r="V6" s="23"/>
       <c r="W6" s="19"/>
       <c r="X6" s="19"/>
@@ -23435,14 +23460,24 @@
     </row>
     <row r="7" spans="1:55" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="21">
+        <v>84</v>
+      </c>
+      <c r="C7" s="23">
+        <v>2</v>
+      </c>
+      <c r="D7" s="23">
+        <v>58</v>
+      </c>
+      <c r="E7" s="24">
+        <v>2</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>48</v>
+      </c>
       <c r="G7" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -23458,7 +23493,9 @@
       <c r="S7" s="23"/>
       <c r="T7" s="23"/>
       <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
+      <c r="V7" s="23">
+        <v>0.5</v>
+      </c>
       <c r="W7" s="19"/>
       <c r="X7" s="19"/>
       <c r="Y7" s="23"/>
@@ -23495,14 +23532,24 @@
     </row>
     <row r="8" spans="1:55" ht="13.5" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="21">
+        <v>84</v>
+      </c>
+      <c r="C8" s="23">
+        <v>2</v>
+      </c>
+      <c r="D8" s="23">
+        <v>58</v>
+      </c>
+      <c r="E8" s="24">
+        <v>3</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>48</v>
+      </c>
       <c r="G8" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
@@ -23519,7 +23566,9 @@
       <c r="T8" s="23"/>
       <c r="U8" s="23"/>
       <c r="V8" s="23"/>
-      <c r="W8" s="19"/>
+      <c r="W8" s="19">
+        <v>2</v>
+      </c>
       <c r="X8" s="19"/>
       <c r="Y8" s="23"/>
       <c r="Z8" s="23"/>
@@ -25184,7 +25233,7 @@
       </c>
       <c r="G36" s="36">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>5.75</v>
       </c>
       <c r="H36" s="37">
         <f t="shared" ref="H36:AL36" si="1">SUM(H3:H35)</f>
@@ -25240,15 +25289,15 @@
       </c>
       <c r="U36" s="72">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="V36" s="72">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="W36" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X36" s="37">
         <f t="shared" si="1"/>

</xml_diff>